<commit_message>
Update whether the additonal fields
</commit_message>
<xml_diff>
--- a/data/additional_tables.xlsx
+++ b/data/additional_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/kate_storey_ontario_ca1/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benhlina/Library/CloudStorage/Dropbox/GitHub/GLATAR-App/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E763AB52-81FA-44AD-A8DC-B2024FB7810F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC4F26D-7AA5-1D42-8E72-EDCB4273714B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4515" yWindow="885" windowWidth="22020" windowHeight="14565" xr2:uid="{86792272-B11E-479C-9F6F-53B61FD5C2BE}"/>
+    <workbookView xWindow="4520" yWindow="880" windowWidth="22020" windowHeight="14560" activeTab="1" xr2:uid="{86792272-B11E-479C-9F6F-53B61FD5C2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -306,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -326,30 +326,29 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -688,20 +687,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B613BDE-8B1A-4C65-A43B-ED774E8653E1}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="49.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="49.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
@@ -718,7 +717,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -733,215 +732,215 @@
       </c>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:5" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:5" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" s="13" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" s="12" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" spans="1:5" s="17" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" s="16" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="15"/>
-    </row>
-    <row r="10" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="15"/>
-    </row>
-    <row r="12" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="15"/>
+      <c r="E16" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -952,30 +951,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB92C68D-174E-45C4-AADE-8120844543EB}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -996,7 +995,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>

</xml_diff>